<commit_message>
CORTES DE LA SEMANA 38
</commit_message>
<xml_diff>
--- a/cosas por pedir/LISTA DE LOS PEDIDOS DE REFACCIONARIA MOTOZOM.xlsx
+++ b/cosas por pedir/LISTA DE LOS PEDIDOS DE REFACCIONARIA MOTOZOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\GitHub\Motozom\cosas por pedir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34105301-8672-4123-9E88-0E226DD85A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D3CECF-CF1E-4F53-9BEF-EBFF08CEC58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
   <si>
     <t xml:space="preserve">LISTA DE PEDIDO SEMANA 15 DE ABRIL </t>
   </si>
@@ -144,15 +144,9 @@
     <t>SELENOIDE FT150</t>
   </si>
   <si>
-    <t>SLAIDER DE DM200</t>
-  </si>
-  <si>
     <t>/</t>
   </si>
   <si>
-    <t>LLANTA 140-70-17</t>
-  </si>
-  <si>
     <t xml:space="preserve">OSCAR </t>
   </si>
   <si>
@@ -165,12 +159,6 @@
     <t xml:space="preserve">BUJIA PARA PULSAR 200NS </t>
   </si>
   <si>
-    <t xml:space="preserve">ACEITE YAMALUBE </t>
-  </si>
-  <si>
-    <t>DESCONOCZCO</t>
-  </si>
-  <si>
     <t>MANGUERA DE FRENO AT110</t>
   </si>
   <si>
@@ -178,6 +166,27 @@
   </si>
   <si>
     <t xml:space="preserve">PORTAFUSIBLES </t>
+  </si>
+  <si>
+    <t>CARBURADOR DS150</t>
+  </si>
+  <si>
+    <t>SLAIDER DM200</t>
+  </si>
+  <si>
+    <t>ACEITE YAMALUBE</t>
+  </si>
+  <si>
+    <t>DESCONOZCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUJIA PULSAR </t>
+  </si>
+  <si>
+    <t>AUXILIAR BUHO</t>
+  </si>
+  <si>
+    <t>BANDA 743-20-30</t>
   </si>
 </sst>
 </file>
@@ -638,7 +647,7 @@
   <dimension ref="B5:P112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +754,9 @@
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="F8" s="1" t="s">
@@ -781,10 +792,10 @@
         <v>10</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>28</v>
@@ -849,7 +860,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>16</v>
@@ -870,7 +881,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>21</v>
@@ -884,8 +895,12 @@
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="F14" s="10" t="s">
         <v>36</v>
@@ -900,7 +915,7 @@
     </row>
     <row r="15" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>2</v>
@@ -916,8 +931,12 @@
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="F16" s="1"/>
       <c r="I16" s="1"/>
@@ -930,9 +949,11 @@
     </row>
     <row r="17" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="F17" s="1"/>
       <c r="I17" s="1"/>
@@ -944,10 +965,14 @@
       <c r="P17" s="1"/>
     </row>
     <row r="18" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="B18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="D18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="1"/>
       <c r="I18" s="1"/>
@@ -959,8 +984,12 @@
       <c r="P18" s="1"/>
     </row>
     <row r="19" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+      <c r="B19" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
       <c r="I19" s="1"/>
@@ -973,7 +1002,7 @@
     </row>
     <row r="20" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>2</v>
@@ -990,7 +1019,7 @@
     </row>
     <row r="21" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>2</v>
@@ -1006,10 +1035,10 @@
       <c r="P21" s="1"/>
     </row>
     <row r="22" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="B22" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="1"/>
@@ -1023,8 +1052,12 @@
       <c r="P22" s="1"/>
     </row>
     <row r="23" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
+      <c r="B23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="F23" s="1"/>
       <c r="I23" s="1"/>
@@ -1037,11 +1070,9 @@
     </row>
     <row r="24" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>47</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C24" s="7"/>
       <c r="D24" s="1"/>
       <c r="F24" s="1"/>
       <c r="I24" s="1"/>
@@ -1066,12 +1097,8 @@
       <c r="P25" s="1"/>
     </row>
     <row r="26" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
       <c r="D26" s="1"/>
       <c r="F26" s="1"/>
       <c r="I26" s="1"/>
@@ -1109,24 +1136,16 @@
       <c r="P28" s="1"/>
     </row>
     <row r="29" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="1"/>
       <c r="F29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>2</v>
-      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="1"/>
       <c r="F30" s="1"/>
       <c r="I30" s="1"/>

</xml_diff>

<commit_message>
SEMANA 39 DE SEPTIEMBRE-25
</commit_message>
<xml_diff>
--- a/cosas por pedir/LISTA DE LOS PEDIDOS DE REFACCIONARIA MOTOZOM.xlsx
+++ b/cosas por pedir/LISTA DE LOS PEDIDOS DE REFACCIONARIA MOTOZOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\GitHub\Motozom\cosas por pedir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D3CECF-CF1E-4F53-9BEF-EBFF08CEC58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1379F66-66BF-4F23-A856-C38549256188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t xml:space="preserve">LISTA DE PEDIDO SEMANA 15 DE ABRIL </t>
   </si>
@@ -187,6 +187,21 @@
   </si>
   <si>
     <t>BANDA 743-20-30</t>
+  </si>
+  <si>
+    <t>PASTAS DE CLUTH PULSAR 200NS</t>
+  </si>
+  <si>
+    <t>CHICOTE DE VELOCIMETRO DM200</t>
+  </si>
+  <si>
+    <t>CENTRIFUJO DS150</t>
+  </si>
+  <si>
+    <t>CADENA 520 SENCILLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUXILIARES </t>
   </si>
 </sst>
 </file>
@@ -647,7 +662,7 @@
   <dimension ref="B5:P112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,8 +1099,12 @@
       <c r="P24" s="1"/>
     </row>
     <row r="25" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
+      <c r="B25" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="F25" s="1"/>
       <c r="I25" s="1"/>
@@ -1097,8 +1116,12 @@
       <c r="P25" s="1"/>
     </row>
     <row r="26" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
+      <c r="B26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D26" s="1"/>
       <c r="F26" s="1"/>
       <c r="I26" s="1"/>
@@ -1110,8 +1133,12 @@
       <c r="P26" s="1"/>
     </row>
     <row r="27" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
+      <c r="B27" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D27" s="1"/>
       <c r="F27" s="1"/>
       <c r="I27" s="1"/>
@@ -1123,8 +1150,12 @@
       <c r="P27" s="1"/>
     </row>
     <row r="28" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+      <c r="B28" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D28" s="1"/>
       <c r="F28" s="1"/>
       <c r="I28" s="1"/>
@@ -1136,8 +1167,12 @@
       <c r="P28" s="1"/>
     </row>
     <row r="29" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
+      <c r="B29" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="D29" s="1"/>
       <c r="F29" s="1"/>
       <c r="I29" s="1"/>

</xml_diff>